<commit_message>
add start date in get page
</commit_message>
<xml_diff>
--- a/web/material/template/gather_template.xlsx
+++ b/web/material/template/gather_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunshine/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunshine/Documents/Itellij/Selling/target/selling-1.0.2-SNAPSHOT/material/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>云草纲目收款单</t>
   </si>
@@ -41,22 +41,10 @@
     <t>订单编号</t>
   </si>
   <si>
-    <t>发货信息</t>
-  </si>
-  <si>
-    <t>发货单号码</t>
-  </si>
-  <si>
     <t>订货金额</t>
   </si>
   <si>
-    <t>发货金额</t>
-  </si>
-  <si>
     <t>订货日期</t>
-  </si>
-  <si>
-    <t>发货日期</t>
   </si>
   <si>
     <t>客户名称</t>
@@ -116,60 +104,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="2">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -181,170 +119,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -357,68 +131,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -701,120 +429,114 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="7" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="7" t="s">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="7" t="s">
+      <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="D3:D5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add selling member in gather template
</commit_message>
<xml_diff>
--- a/web/material/template/gather_template.xlsx
+++ b/web/material/template/gather_template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>云草纲目收款单</t>
   </si>
@@ -74,6 +74,9 @@
   <si>
     <t>渠道</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售员</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -142,11 +145,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -155,6 +195,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -164,7 +205,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,31 +492,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
@@ -479,52 +529,52 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
@@ -539,15 +589,26 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="C9:F9"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C2:D2"/>

</xml_diff>